<commit_message>
update to Jul 10th.
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelxu/My_Document/Michael/金融/量化/Prediction/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD89043-B6DB-4241-B3AC-12F1F3F8C741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A26446B-74C4-2F42-A0BA-8449A1430564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="500" windowWidth="15360" windowHeight="17720" xr2:uid="{49E41F07-E01F-DB49-9AD6-EC869743E72B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="18700" xr2:uid="{49E41F07-E01F-DB49-9AD6-EC869743E72B}"/>
   </bookViews>
   <sheets>
     <sheet name="Watchlist" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="373">
   <si>
     <t>603993.SS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1204,6 +1204,10 @@
   </si>
   <si>
     <t>600938.SS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>603799.SS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1652,10 +1656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F422F51A-3928-6949-A930-8426377A892F}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1685,7 +1689,7 @@
       </c>
       <c r="E1" s="1">
         <f ca="1">TODAY()</f>
-        <v>45475</v>
+        <v>45483</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>341</v>
@@ -1699,478 +1703,499 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>366</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B17" si="0">SUBSTITUTE(A2,"SS","SH")</f>
-        <v>601225.SH</v>
+        <f>SUBSTITUTE(A2,"SS","SH")</f>
+        <v>002299.SZ</v>
       </c>
       <c r="C2" t="str">
         <f>[1]!s_info_name(B2)</f>
-        <v>陕西煤业</v>
+        <v>圣农发展</v>
       </c>
       <c r="D2" s="2">
         <f ca="1">[1]!s_val_mv_ref(B2,$E$1,100000000)</f>
-        <v>2598.2600000000002</v>
+        <v>153.43559640000001</v>
       </c>
       <c r="F2" t="str">
         <f>[1]!s_info_thematicindustry_wind(B2,"")</f>
-        <v>煤炭</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="H2" t="s">
-        <v>346</v>
+        <v>食品</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>371</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" si="0"/>
-        <v>601898.SH</v>
+        <f>SUBSTITUTE(A3,"SS","SH")</f>
+        <v>600938.SH</v>
       </c>
       <c r="C3" t="str">
         <f>[1]!s_info_name(B3)</f>
-        <v>中煤能源</v>
+        <v>中国海油</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">[1]!s_val_mv_ref(B3,$E$1,100000000)</f>
-        <v>1706.38997958</v>
+        <v>16120.376314179999</v>
       </c>
       <c r="F3" t="str">
         <f>[1]!s_info_thematicindustry_wind(B3,"")</f>
-        <v>煤炭</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="H3" t="s">
-        <v>348</v>
+        <v>石油天然气</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>603993.SH</v>
+        <f>SUBSTITUTE(A4,"SS","SH")</f>
+        <v>601225.SH</v>
       </c>
       <c r="C4" t="str">
         <f>[1]!s_info_name(B4)</f>
-        <v>洛阳钼业</v>
+        <v>陕西煤业</v>
       </c>
       <c r="D4" s="2">
         <f ca="1">[1]!s_val_mv_ref(B4,$E$1,100000000)</f>
-        <v>1844.5751457900001</v>
+        <v>2462.5300000000002</v>
       </c>
       <c r="F4" t="str">
         <f>[1]!s_info_thematicindustry_wind(B4,"")</f>
-        <v>基本金属</v>
+        <v>煤炭</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>600111.SH</v>
-      </c>
-      <c r="C5" s="5" t="str">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="str">
+        <f>SUBSTITUTE(A5,"SS","SH")</f>
+        <v>601898.SH</v>
+      </c>
+      <c r="C5" t="str">
         <f>[1]!s_info_name(B5)</f>
-        <v>北方稀土</v>
+        <v>中煤能源</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">[1]!s_val_mv_ref(B5,$E$1,100000000)</f>
-        <v>634.44405527000004</v>
+        <v>1608.27587042</v>
       </c>
       <c r="F5" t="str">
         <f>[1]!s_info_thematicindustry_wind(B5,"")</f>
-        <v>基本金属</v>
+        <v>煤炭</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>343</v>
       </c>
       <c r="H5" t="s">
-        <v>350</v>
-      </c>
-      <c r="I5" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>000831.SZ</v>
-      </c>
-      <c r="C6" s="5" t="str">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="str">
+        <f>SUBSTITUTE(A6,"SS","SH")</f>
+        <v>603993.SH</v>
+      </c>
+      <c r="C6" t="str">
         <f>[1]!s_info_name(B6)</f>
-        <v>中国稀土</v>
+        <v>洛阳钼业</v>
       </c>
       <c r="D6" s="2">
         <f ca="1">[1]!s_val_mv_ref(B6,$E$1,100000000)</f>
-        <v>267.42764335999999</v>
+        <v>1896.41332319</v>
       </c>
       <c r="F6" t="str">
         <f>[1]!s_info_thematicindustry_wind(B6,"")</f>
         <v>基本金属</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H6" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>364</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>601919.SH</v>
-      </c>
-      <c r="C7" t="str">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <f>SUBSTITUTE(A7,"SS","SH")</f>
+        <v>600111.SH</v>
+      </c>
+      <c r="C7" s="5" t="str">
         <f>[1]!s_info_name(B7)</f>
-        <v>中远海控</v>
+        <v>北方稀土</v>
       </c>
       <c r="D7" s="2">
         <f ca="1">[1]!s_val_mv_ref(B7,$E$1,100000000)</f>
-        <v>2561.66720751</v>
+        <v>615.28420630999995</v>
       </c>
       <c r="F7" t="str">
         <f>[1]!s_info_thematicindustry_wind(B7,"")</f>
-        <v>海运</v>
+        <v>基本金属</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="H7" t="s">
+        <v>350</v>
+      </c>
+      <c r="I7" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>600026.SH</v>
-      </c>
-      <c r="C8" t="str">
+      <c r="A8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="str">
+        <f>SUBSTITUTE(A8,"SS","SH")</f>
+        <v>000831.SZ</v>
+      </c>
+      <c r="C8" s="5" t="str">
         <f>[1]!s_info_name(B8)</f>
-        <v>中远海能</v>
+        <v>中国稀土</v>
       </c>
       <c r="D8" s="2">
         <f ca="1">[1]!s_val_mv_ref(B8,$E$1,100000000)</f>
-        <v>754.25974804999998</v>
+        <v>252.67667415</v>
       </c>
       <c r="F8" t="str">
         <f>[1]!s_info_thematicindustry_wind(B8,"")</f>
-        <v>海运</v>
+        <v>基本金属</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>344</v>
       </c>
       <c r="H8" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>000975.SZ</v>
+        <f>SUBSTITUTE(A9,"SS","SH")</f>
+        <v>002460.SZ</v>
       </c>
       <c r="C9" t="str">
         <f>[1]!s_info_name(B9)</f>
-        <v>银泰黄金</v>
+        <v>赣锋锂业</v>
       </c>
       <c r="D9" s="2">
         <f ca="1">[1]!s_val_mv_ref(B9,$E$1,100000000)</f>
-        <v>468.15537388000001</v>
+        <v>561.17607611999995</v>
       </c>
       <c r="F9" t="str">
         <f>[1]!s_info_thematicindustry_wind(B9,"")</f>
-        <v>贵金属</v>
+        <v>基本金属</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>002155.SZ</v>
-      </c>
-      <c r="C10" s="5" t="str">
+      <c r="A10" t="s">
+        <v>368</v>
+      </c>
+      <c r="B10" t="str">
+        <f>SUBSTITUTE(A10,"SS","SH")</f>
+        <v>002466.SZ</v>
+      </c>
+      <c r="C10" t="str">
         <f>[1]!s_info_name(B10)</f>
-        <v>湖南黄金</v>
+        <v>天齐锂业</v>
       </c>
       <c r="D10" s="2">
         <f ca="1">[1]!s_val_mv_ref(B10,$E$1,100000000)</f>
-        <v>227.78648032000001</v>
+        <v>458.22906597000002</v>
       </c>
       <c r="F10" t="str">
         <f>[1]!s_info_thematicindustry_wind(B10,"")</f>
-        <v>贵金属</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="H10" t="s">
-        <v>348</v>
+        <v>基本金属</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="B11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>600301.SH</v>
-      </c>
-      <c r="C11" s="5" t="str">
+      <c r="A11" t="s">
+        <v>369</v>
+      </c>
+      <c r="B11" t="str">
+        <f>SUBSTITUTE(A11,"SS","SH")</f>
+        <v>601600.SH</v>
+      </c>
+      <c r="C11" t="str">
         <f>[1]!s_info_name(B11)</f>
-        <v>华锡有色</v>
+        <v>中国铝业</v>
       </c>
       <c r="D11" s="2">
         <f ca="1">[1]!s_val_mv_ref(B11,$E$1,100000000)</f>
-        <v>127.46234702</v>
+        <v>1297.17362084</v>
       </c>
       <c r="F11" t="str">
         <f>[1]!s_info_thematicindustry_wind(B11,"")</f>
-        <v>贵金属</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="H11" t="s">
-        <v>348</v>
-      </c>
-      <c r="I11" t="s">
-        <v>354</v>
+        <v>基本金属</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>372</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>601298.SH</v>
+        <f>SUBSTITUTE(A12,"SS","SH")</f>
+        <v>603799.SH</v>
       </c>
       <c r="C12" t="str">
         <f>[1]!s_info_name(B12)</f>
-        <v>青岛港</v>
+        <v>华友钴业</v>
       </c>
       <c r="D12" s="2">
         <f ca="1">[1]!s_val_mv_ref(B12,$E$1,100000000)</f>
-        <v>625.74203999999997</v>
+        <v>394.77172495999997</v>
       </c>
       <c r="F12" t="str">
         <f>[1]!s_info_thematicindustry_wind(B12,"")</f>
-        <v>港口</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="H12" t="s">
-        <v>348</v>
+        <v>基本金属</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>364</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>600895.SH</v>
+        <f>SUBSTITUTE(A13,"SS","SH")</f>
+        <v>601919.SH</v>
       </c>
       <c r="C13" t="str">
         <f>[1]!s_info_name(B13)</f>
-        <v>张江高科</v>
+        <v>中远海控</v>
       </c>
       <c r="D13" s="2">
         <f ca="1">[1]!s_val_mv_ref(B13,$E$1,100000000)</f>
-        <v>284.64913928999999</v>
+        <v>2293.5390771699999</v>
       </c>
       <c r="F13" t="str">
         <f>[1]!s_info_thematicindustry_wind(B13,"")</f>
-        <v>房地产</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="H13" t="s">
-        <v>351</v>
+        <v>海运</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>601985.SH</v>
+        <f>SUBSTITUTE(A14,"SS","SH")</f>
+        <v>600026.SH</v>
       </c>
       <c r="C14" t="str">
         <f>[1]!s_info_name(B14)</f>
-        <v>中国核电</v>
+        <v>中远海能</v>
       </c>
       <c r="D14" s="2">
         <f ca="1">[1]!s_val_mv_ref(B14,$E$1,100000000)</f>
-        <v>2077.16133537</v>
+        <v>694.62504310999998</v>
       </c>
       <c r="F14" t="str">
         <f>[1]!s_info_thematicindustry_wind(B14,"")</f>
-        <v>电力</v>
+        <v>海运</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="H14" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>002299.SZ</v>
+        <f>SUBSTITUTE(A15,"SS","SH")</f>
+        <v>000975.SZ</v>
       </c>
       <c r="C15" t="str">
         <f>[1]!s_info_name(B15)</f>
-        <v>圣农发展</v>
+        <v>银泰黄金</v>
       </c>
       <c r="D15" s="2">
         <f ca="1">[1]!s_val_mv_ref(B15,$E$1,100000000)</f>
-        <v>166.11827941000001</v>
+        <v>491.20216868</v>
       </c>
       <c r="F15" t="str">
         <f>[1]!s_info_thematicindustry_wind(B15,"")</f>
-        <v>食品</v>
+        <v>贵金属</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>367</v>
-      </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>002460.SZ</v>
-      </c>
-      <c r="C16" t="str">
+      <c r="A16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5" t="str">
+        <f>SUBSTITUTE(A16,"SS","SH")</f>
+        <v>002155.SZ</v>
+      </c>
+      <c r="C16" s="5" t="str">
         <f>[1]!s_info_name(B16)</f>
-        <v>赣锋锂业</v>
+        <v>湖南黄金</v>
       </c>
       <c r="D16" s="2">
         <f ca="1">[1]!s_val_mv_ref(B16,$E$1,100000000)</f>
-        <v>575.09453379000001</v>
+        <v>220.09342769</v>
       </c>
       <c r="F16" t="str">
         <f>[1]!s_info_thematicindustry_wind(B16,"")</f>
-        <v>基本金属</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>368</v>
-      </c>
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>002466.SZ</v>
-      </c>
-      <c r="C17" t="str">
+        <v>贵金属</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="H16" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B17" s="5" t="str">
+        <f>SUBSTITUTE(A17,"SS","SH")</f>
+        <v>600301.SH</v>
+      </c>
+      <c r="C17" s="5" t="str">
         <f>[1]!s_info_name(B17)</f>
-        <v>天齐锂业</v>
+        <v>华锡有色</v>
       </c>
       <c r="D17" s="2">
         <f ca="1">[1]!s_val_mv_ref(B17,$E$1,100000000)</f>
-        <v>483.33975619</v>
+        <v>121.45295597</v>
       </c>
       <c r="F17" t="str">
         <f>[1]!s_info_thematicindustry_wind(B17,"")</f>
-        <v>基本金属</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>贵金属</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="H17" t="s">
+        <v>348</v>
+      </c>
+      <c r="I17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>369</v>
+        <v>14</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" ref="B18:B20" si="1">SUBSTITUTE(A18,"SS","SH")</f>
-        <v>601600.SH</v>
+        <f>SUBSTITUTE(A18,"SS","SH")</f>
+        <v>601298.SH</v>
       </c>
       <c r="C18" t="str">
         <f>[1]!s_info_name(B18)</f>
-        <v>中国铝业</v>
+        <v>青岛港</v>
       </c>
       <c r="D18" s="2">
         <f ca="1">[1]!s_val_mv_ref(B18,$E$1,100000000)</f>
-        <v>1338.3537357800001</v>
+        <v>641.96978999999999</v>
       </c>
       <c r="F18" t="str">
         <f>[1]!s_info_thematicindustry_wind(B18,"")</f>
-        <v>基本金属</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>港口</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="H18" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>370</v>
+        <v>4</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="1"/>
-        <v>600900.SH</v>
+        <f>SUBSTITUTE(A19,"SS","SH")</f>
+        <v>600895.SH</v>
       </c>
       <c r="C19" t="str">
         <f>[1]!s_info_name(B19)</f>
-        <v>长江电力</v>
+        <v>张江高科</v>
       </c>
       <c r="D19" s="2">
         <f ca="1">[1]!s_val_mv_ref(B19,$E$1,100000000)</f>
-        <v>7213.2305826800002</v>
+        <v>281.08715332999998</v>
       </c>
       <c r="F19" t="str">
         <f>[1]!s_info_thematicindustry_wind(B19,"")</f>
-        <v>电力</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>房地产</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="H19" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>371</v>
+        <v>13</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="1"/>
-        <v>600938.SH</v>
+        <f>SUBSTITUTE(A20,"SS","SH")</f>
+        <v>601985.SH</v>
       </c>
       <c r="C20" t="str">
         <f>[1]!s_info_name(B20)</f>
-        <v>中国海油</v>
+        <v>中国核电</v>
       </c>
       <c r="D20" s="2">
         <f ca="1">[1]!s_val_mv_ref(B20,$E$1,100000000)</f>
-        <v>16714.960863979999</v>
+        <v>2122.4812190500002</v>
       </c>
       <c r="F20" t="str">
         <f>[1]!s_info_thematicindustry_wind(B20,"")</f>
-        <v>石油天然气</v>
+        <v>电力</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="H20" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>370</v>
+      </c>
+      <c r="B21" t="str">
+        <f>SUBSTITUTE(A21,"SS","SH")</f>
+        <v>600900.SH</v>
+      </c>
+      <c r="C21" t="str">
+        <f>[1]!s_info_name(B21)</f>
+        <v>长江电力</v>
+      </c>
+      <c r="D21" s="2">
+        <f ca="1">[1]!s_val_mv_ref(B21,$E$1,100000000)</f>
+        <v>7364.93353252</v>
+      </c>
+      <c r="F21" t="str">
+        <f>[1]!s_info_thematicindustry_wind(B21,"")</f>
+        <v>电力</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I14">
-    <sortCondition descending="1" ref="F1:F14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I21">
+    <sortCondition descending="1" ref="F1:F21"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E2:E7">
@@ -2233,7 +2258,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H14 F2:L2 G3:L5 G7:L7 H6:L6 F3:F20">
+  <conditionalFormatting sqref="H8:H14 F2:L2 G3:L5 G7:L7 H6:L6 F3:F21">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>